<commit_message>
📝 add research report
</commit_message>
<xml_diff>
--- a/data/scatter-data.xlsx
+++ b/data/scatter-data.xlsx
@@ -5,24 +5,99 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/glamour/data/run00/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/glamour/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B39D238-33DF-BC40-973C-D9E04099AA30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86382AFC-FD51-FD47-9164-9D4DAF9A3098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="1240" windowWidth="28800" windowHeight="16260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="run00" sheetId="1" r:id="rId1"/>
     <sheet name="run01" sheetId="3" r:id="rId2"/>
     <sheet name="run02" sheetId="5" r:id="rId3"/>
+    <sheet name="run03" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'run03'!$D$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'run03'!$D$2:$D$51</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'run03'!$E$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'run03'!$E$2:$E$51</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'run03'!$D$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'run03'!$D$2:$D$51</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'run03'!$E$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'run03'!$E$2:$E$51</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">'run03'!$B$2:$B$251</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'run03'!$A$1</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">'run03'!$C$1</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">'run03'!$C$2:$C$251</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'run03'!$A$2:$A$251</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'run03'!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'run03'!$B$2:$B$251</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>min</t>
   </si>
@@ -31,6 +106,12 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>avg/min</t>
+  </si>
+  <si>
+    <t>max/avg</t>
   </si>
 </sst>
 </file>
@@ -8935,6 +9016,1611 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'run03'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'run03'!$A$2:$A$251</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="250"/>
+                <c:pt idx="0">
+                  <c:v>3333400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3333378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3333388</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4956730</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27910872</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3330164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3333490</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3333226</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7929630</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32618952</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3333237</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3333358</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3333303</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38573035</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113376605</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3333004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3333733</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3341002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>118402484</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>330656582</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3332733</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3333315</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3340778</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>344543184</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>912672550</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3332782</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3333159</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3332977</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5933801</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29196583</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3333118</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3333297</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3332432</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9063973</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35112622</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17260657</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3336435</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3333828</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5600161</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43936360</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>52678362</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3333739</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3350932</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5920143</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>83091854</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>134695479</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>132944730</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>135582178</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>140975194</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>174880377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE19-A749-B9CA-2CED78DE3CC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'run03'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'run03'!$B$2:$B$251</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="250"/>
+                <c:pt idx="0">
+                  <c:v>3508624</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3503090</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3394145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6405593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30017652</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53269932</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3485312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3479624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10788166</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34970334</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3478768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3371851</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32700345</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42248249</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120017429</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3368786</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>77577666</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99495628</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>125087299</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>341476958</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3524289</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28709836</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>96427123</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>356602594</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>912672550</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3348864</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3374808</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3538749</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21524405</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39673661</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31476296</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37010872</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24817865</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12260164</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38120969</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19470855</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>132907023</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76838384</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40768613</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>54033737</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>55236886</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>382217655</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>219124438</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>111353347</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>84955928</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>138703348</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>138898976</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>270626137</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>144129043</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>177765368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AE19-A749-B9CA-2CED78DE3CC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'run03'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'run03'!$C$2:$C$251</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="250"/>
+                <c:pt idx="0">
+                  <c:v>3339428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3339712</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3339213</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5561731</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29159187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3591565</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3339783</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3339425</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9064394</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33390051</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3338963</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3338318</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6513392</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40159530</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>116978969</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3338665</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14687106</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27497440</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121400110</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>336928584</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3342311</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3590316</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48864434</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>351093078</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>912672550</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3338272</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3339088</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3342647</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8229011</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32725063</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4781756</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5053198</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5770058</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10678923</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36422114</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18280655</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18332806</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19099024</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>24198861</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49376229</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>53914765</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>54188749</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>54695925</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>59538425</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>83933094</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>136766750</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>136180223</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>157031598</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>142376131</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>176125589</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AE19-A749-B9CA-2CED78DE3CC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="258367824"/>
+        <c:axId val="258411888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="258367824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Config Num.</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="258411888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="258411888"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000000"/>
+          <c:min val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frame Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="258367824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200" baseline="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'run03'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg/min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'run03'!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0018083638327233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0019001745376612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00174747134147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1220564767497927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0447250447782499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0784949329822795</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0018878112728702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0018597598842682</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.143104281032028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0236396006836761</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0017178496458548</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0014879889888815</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9540353817219738</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0411296388785585</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0317734333286837</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0016984678086196</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.4056035681321806</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.2302973778525121</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0253172560129735</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0189683264795859</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0028739175925585</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0771007240539823</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.626663010831608</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0190103717158427</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0016472724588648</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0017787930308755</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.002901310150055</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3868026581949748</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1208524983899657</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4346194764181766</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5159759241375732</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.7314855937045377</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1781724195339063</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0372940534033601</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0590938108555197</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.4947289547076448</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.7288570376156178</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.3211009469192048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.1238124642095977</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0234707943272801</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.254646509519791</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>16.322600697358226</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10.056923456071923</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0101242174714262</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.0153774351995883</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0243371286699368</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.1582023560648214</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0099374716944882</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.0071203643391047</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D7B-774F-BF1B-185D1DCCED93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'run03'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max/avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'run03'!$E$2:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0506661619894186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0489197870954141</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0164505828169692</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1517265038528472</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0294406356391212</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.831955428900772</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0435743879168198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0419829761111568</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1901695800072238</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0473279600561256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0418707844321724</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0100448788881107</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0204785770609233</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0520105439480989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0259744125458996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0090218695197033</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.282025335692409</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6183596727549912</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0303722047698309</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0134995195302279</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0544467585452102</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.9964649351199171</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.9733600720720514</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0156924654606834</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0031728990327931</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0106975317811331</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.0586666794310018</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.615673378003748</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.2123326088020059</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.5825809597980323</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.3242473380223769</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.3011465396015085</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1480712053078761</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.04664350344958</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0651070763055261</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.2496825090496237</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.0231576231329935</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.6847327235773617</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.094326928044667</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0245224290600172</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.0534504311955972</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.0062296779878936</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.8702770017849817</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0121863016273414</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.0141598597612358</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0199643747095348</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7233865059438547</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0123118389837409</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.0093102825620643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D7B-774F-BF1B-185D1DCCED93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1509022399"/>
+        <c:axId val="1508991503"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1509022399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1508991503"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1508991503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1509022399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -9013,6 +10699,83 @@
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -10594,6 +12357,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10713,6 +13508,85 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>332317</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>60111</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4D12E98-9C09-894F-BD8B-8B3B7137FE3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>696360</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>26826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>488022</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>172947</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A082510D-B57D-DC44-90B9-6D34AEA82E79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10982,7 +13856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -16538,7 +19412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090AB1B8-A1E0-AB43-8D36-A9E0FEFEB145}">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
@@ -19310,4 +22184,988 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A572B5-19C2-4047-B25A-4B31E0C745F4}">
+  <dimension ref="A1:E51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3333400</v>
+      </c>
+      <c r="B2">
+        <v>3508624</v>
+      </c>
+      <c r="C2">
+        <v>3339428</v>
+      </c>
+      <c r="D2">
+        <f>C2/A2</f>
+        <v>1.0018083638327233</v>
+      </c>
+      <c r="E2">
+        <f>B2/C2</f>
+        <v>1.0506661619894186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3333378</v>
+      </c>
+      <c r="B3">
+        <v>3503090</v>
+      </c>
+      <c r="C3">
+        <v>3339712</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D51" si="0">C3/A3</f>
+        <v>1.0019001745376612</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E51" si="1">B3/C3</f>
+        <v>1.0489197870954141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3333388</v>
+      </c>
+      <c r="B4">
+        <v>3394145</v>
+      </c>
+      <c r="C4">
+        <v>3339213</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.00174747134147</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1.0164505828169692</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4956730</v>
+      </c>
+      <c r="B5">
+        <v>6405593</v>
+      </c>
+      <c r="C5">
+        <v>5561731</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.1220564767497927</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1.1517265038528472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>27910872</v>
+      </c>
+      <c r="B6">
+        <v>30017652</v>
+      </c>
+      <c r="C6">
+        <v>29159187</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.0447250447782499</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1.0294406356391212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3330164</v>
+      </c>
+      <c r="B7">
+        <v>53269932</v>
+      </c>
+      <c r="C7">
+        <v>3591565</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.0784949329822795</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>14.831955428900772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3333490</v>
+      </c>
+      <c r="B8">
+        <v>3485312</v>
+      </c>
+      <c r="C8">
+        <v>3339783</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.0018878112728702</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>1.0435743879168198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3333226</v>
+      </c>
+      <c r="B9">
+        <v>3479624</v>
+      </c>
+      <c r="C9">
+        <v>3339425</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.0018597598842682</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.0419829761111568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7929630</v>
+      </c>
+      <c r="B10">
+        <v>10788166</v>
+      </c>
+      <c r="C10">
+        <v>9064394</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.143104281032028</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1.1901695800072238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>32618952</v>
+      </c>
+      <c r="B11">
+        <v>34970334</v>
+      </c>
+      <c r="C11">
+        <v>33390051</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.0236396006836761</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>1.0473279600561256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3333237</v>
+      </c>
+      <c r="B12">
+        <v>3478768</v>
+      </c>
+      <c r="C12">
+        <v>3338963</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.0017178496458548</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1.0418707844321724</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3333358</v>
+      </c>
+      <c r="B13">
+        <v>3371851</v>
+      </c>
+      <c r="C13">
+        <v>3338318</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.0014879889888815</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.0100448788881107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3333303</v>
+      </c>
+      <c r="B14">
+        <v>32700345</v>
+      </c>
+      <c r="C14">
+        <v>6513392</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.9540353817219738</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>5.0204785770609233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>38573035</v>
+      </c>
+      <c r="B15">
+        <v>42248249</v>
+      </c>
+      <c r="C15">
+        <v>40159530</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.0411296388785585</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>1.0520105439480989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>113376605</v>
+      </c>
+      <c r="B16">
+        <v>120017429</v>
+      </c>
+      <c r="C16">
+        <v>116978969</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.0317734333286837</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>1.0259744125458996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3333004</v>
+      </c>
+      <c r="B17">
+        <v>3368786</v>
+      </c>
+      <c r="C17">
+        <v>3338665</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.0016984678086196</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1.0090218695197033</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3333733</v>
+      </c>
+      <c r="B18">
+        <v>77577666</v>
+      </c>
+      <c r="C18">
+        <v>14687106</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>4.4056035681321806</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>5.282025335692409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3341002</v>
+      </c>
+      <c r="B19">
+        <v>99495628</v>
+      </c>
+      <c r="C19">
+        <v>27497440</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>8.2302973778525121</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>3.6183596727549912</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>118402484</v>
+      </c>
+      <c r="B20">
+        <v>125087299</v>
+      </c>
+      <c r="C20">
+        <v>121400110</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.0253172560129735</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>1.0303722047698309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>330656582</v>
+      </c>
+      <c r="B21">
+        <v>341476958</v>
+      </c>
+      <c r="C21">
+        <v>336928584</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1.0189683264795859</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>1.0134995195302279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3332733</v>
+      </c>
+      <c r="B22">
+        <v>3524289</v>
+      </c>
+      <c r="C22">
+        <v>3342311</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1.0028739175925585</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>1.0544467585452102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3333315</v>
+      </c>
+      <c r="B23">
+        <v>28709836</v>
+      </c>
+      <c r="C23">
+        <v>3590316</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1.0771007240539823</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>7.9964649351199171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3340778</v>
+      </c>
+      <c r="B24">
+        <v>96427123</v>
+      </c>
+      <c r="C24">
+        <v>48864434</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>14.626663010831608</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>1.9733600720720514</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>344543184</v>
+      </c>
+      <c r="B25">
+        <v>356602594</v>
+      </c>
+      <c r="C25">
+        <v>351093078</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.0190103717158427</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>1.0156924654606834</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>912672550</v>
+      </c>
+      <c r="B26">
+        <v>912672550</v>
+      </c>
+      <c r="C26">
+        <v>912672550</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3332782</v>
+      </c>
+      <c r="B27">
+        <v>3348864</v>
+      </c>
+      <c r="C27">
+        <v>3338272</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.0016472724588648</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>1.0031728990327931</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3333159</v>
+      </c>
+      <c r="B28">
+        <v>3374808</v>
+      </c>
+      <c r="C28">
+        <v>3339088</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>1.0017787930308755</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>1.0106975317811331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3332977</v>
+      </c>
+      <c r="B29">
+        <v>3538749</v>
+      </c>
+      <c r="C29">
+        <v>3342647</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1.002901310150055</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1.0586666794310018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5933801</v>
+      </c>
+      <c r="B30">
+        <v>21524405</v>
+      </c>
+      <c r="C30">
+        <v>8229011</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1.3868026581949748</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>2.615673378003748</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29196583</v>
+      </c>
+      <c r="B31">
+        <v>39673661</v>
+      </c>
+      <c r="C31">
+        <v>32725063</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1.1208524983899657</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1.2123326088020059</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3333118</v>
+      </c>
+      <c r="B32">
+        <v>31476296</v>
+      </c>
+      <c r="C32">
+        <v>4781756</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1.4346194764181766</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>6.5825809597980323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3333297</v>
+      </c>
+      <c r="B33">
+        <v>37010872</v>
+      </c>
+      <c r="C33">
+        <v>5053198</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1.5159759241375732</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>7.3242473380223769</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3332432</v>
+      </c>
+      <c r="B34">
+        <v>24817865</v>
+      </c>
+      <c r="C34">
+        <v>5770058</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>1.7314855937045377</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>4.3011465396015085</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>9063973</v>
+      </c>
+      <c r="B35">
+        <v>12260164</v>
+      </c>
+      <c r="C35">
+        <v>10678923</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1.1781724195339063</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>1.1480712053078761</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35112622</v>
+      </c>
+      <c r="B36">
+        <v>38120969</v>
+      </c>
+      <c r="C36">
+        <v>36422114</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1.0372940534033601</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>1.04664350344958</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>17260657</v>
+      </c>
+      <c r="B37">
+        <v>19470855</v>
+      </c>
+      <c r="C37">
+        <v>18280655</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>1.0590938108555197</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>1.0651070763055261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3336435</v>
+      </c>
+      <c r="B38">
+        <v>132907023</v>
+      </c>
+      <c r="C38">
+        <v>18332806</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>5.4947289547076448</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>7.2496825090496237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3333828</v>
+      </c>
+      <c r="B39">
+        <v>76838384</v>
+      </c>
+      <c r="C39">
+        <v>19099024</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>5.7288570376156178</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>4.0231576231329935</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>5600161</v>
+      </c>
+      <c r="B40">
+        <v>40768613</v>
+      </c>
+      <c r="C40">
+        <v>24198861</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>4.3211009469192048</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1.6847327235773617</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>43936360</v>
+      </c>
+      <c r="B41">
+        <v>54033737</v>
+      </c>
+      <c r="C41">
+        <v>49376229</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>1.1238124642095977</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>1.094326928044667</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>52678362</v>
+      </c>
+      <c r="B42">
+        <v>55236886</v>
+      </c>
+      <c r="C42">
+        <v>53914765</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>1.0234707943272801</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1.0245224290600172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3333739</v>
+      </c>
+      <c r="B43">
+        <v>382217655</v>
+      </c>
+      <c r="C43">
+        <v>54188749</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>16.254646509519791</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>7.0534504311955972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3350932</v>
+      </c>
+      <c r="B44">
+        <v>219124438</v>
+      </c>
+      <c r="C44">
+        <v>54695925</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>16.322600697358226</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>4.0062296779878936</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5920143</v>
+      </c>
+      <c r="B45">
+        <v>111353347</v>
+      </c>
+      <c r="C45">
+        <v>59538425</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>10.056923456071923</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>1.8702770017849817</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>83091854</v>
+      </c>
+      <c r="B46">
+        <v>84955928</v>
+      </c>
+      <c r="C46">
+        <v>83933094</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>1.0101242174714262</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1.0121863016273414</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>134695479</v>
+      </c>
+      <c r="B47">
+        <v>138703348</v>
+      </c>
+      <c r="C47">
+        <v>136766750</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>1.0153774351995883</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>1.0141598597612358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>132944730</v>
+      </c>
+      <c r="B48">
+        <v>138898976</v>
+      </c>
+      <c r="C48">
+        <v>136180223</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>1.0243371286699368</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>1.0199643747095348</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>135582178</v>
+      </c>
+      <c r="B49">
+        <v>270626137</v>
+      </c>
+      <c r="C49">
+        <v>157031598</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>1.1582023560648214</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>1.7233865059438547</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>140975194</v>
+      </c>
+      <c r="B50">
+        <v>144129043</v>
+      </c>
+      <c r="C50">
+        <v>142376131</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>1.0099374716944882</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>1.0123118389837409</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>174880377</v>
+      </c>
+      <c r="B51">
+        <v>177765368</v>
+      </c>
+      <c r="C51">
+        <v>176125589</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>1.0071203643391047</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>1.0093102825620643</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>